<commit_message>
Test Commit: Added test for checking the higher fullhouse and cardfile line. (also updated grid)
</commit_message>
<xml_diff>
--- a/TottenKyle-grid.xlsx
+++ b/TottenKyle-grid.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktotten\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktotten\workspace\4004A1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="140">
   <si>
     <t>yes/no</t>
   </si>
@@ -501,6 +501,15 @@
   </si>
   <si>
     <t>Lines 56-59</t>
+  </si>
+  <si>
+    <t>Line 60</t>
+  </si>
+  <si>
+    <t>Line 61</t>
+  </si>
+  <si>
+    <t>Line 62</t>
   </si>
 </sst>
 </file>
@@ -1435,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2748,13 +2757,15 @@
         <v>25</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C81" s="6"/>
       <c r="D81">
         <v>0.5</v>
       </c>
-      <c r="E81" s="2"/>
+      <c r="E81" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
@@ -2769,13 +2780,15 @@
         <v>24</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C82" s="6"/>
       <c r="D82">
         <v>0.5</v>
       </c>
-      <c r="E82" s="2"/>
+      <c r="E82" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
@@ -2790,13 +2803,15 @@
         <v>21</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83">
         <v>0.5</v>
       </c>
-      <c r="E83" s="2"/>
+      <c r="E83" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>

</xml_diff>

<commit_message>
Administrative Commit: Pushing the Grid
</commit_message>
<xml_diff>
--- a/TottenKyle-grid.xlsx
+++ b/TottenKyle-grid.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="143">
   <si>
     <t>yes/no</t>
   </si>
@@ -494,22 +494,31 @@
     <t>Totten</t>
   </si>
   <si>
-    <t>yes/no (USE HIGH CARD)</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Lines 56-59</t>
-  </si>
-  <si>
-    <t>Line 60</t>
-  </si>
-  <si>
     <t>Line 61</t>
   </si>
   <si>
     <t>Line 62</t>
+  </si>
+  <si>
+    <t>Line 64</t>
+  </si>
+  <si>
+    <t>Line 63</t>
+  </si>
+  <si>
+    <t>Lines 57-60</t>
+  </si>
+  <si>
+    <t>DetectionTests/threeSuitTest</t>
+  </si>
+  <si>
+    <t>DetectionTests/oneOffRoyalTest</t>
+  </si>
+  <si>
+    <t>Line 67</t>
   </si>
 </sst>
 </file>
@@ -1444,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1601,7 +1610,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13">
@@ -1837,13 +1846,15 @@
         <v>90</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1951,13 +1962,15 @@
         <v>94</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="E33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -2055,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40">
@@ -2092,7 +2105,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43">
@@ -2741,7 +2754,7 @@
         <v>0.5</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
@@ -2764,7 +2777,7 @@
         <v>0.5</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
@@ -2787,7 +2800,7 @@
         <v>0.5</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -2810,7 +2823,7 @@
         <v>0.5</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
@@ -2826,13 +2839,15 @@
         <v>22</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84">
         <v>0.5</v>
       </c>
-      <c r="E84" s="2"/>
+      <c r="E84" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
@@ -2874,13 +2889,15 @@
         <v>27</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C87" s="6"/>
       <c r="D87">
         <v>0.5</v>
       </c>
-      <c r="E87" s="2"/>
+      <c r="E87" s="2">
+        <v>66</v>
+      </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
@@ -2895,13 +2912,15 @@
         <v>28</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C88" s="6"/>
       <c r="D88">
         <v>0.5</v>
       </c>
-      <c r="E88" s="2"/>
+      <c r="E88" s="2">
+        <v>65</v>
+      </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
@@ -3033,13 +3052,15 @@
         <v>38</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C98" s="6"/>
       <c r="D98">
         <v>0.5</v>
       </c>
-      <c r="E98" s="2"/>
+      <c r="E98" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>

</xml_diff>

<commit_message>
Administrative Commit: Updated the Grid
</commit_message>
<xml_diff>
--- a/TottenKyle-grid.xlsx
+++ b/TottenKyle-grid.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktotten\workspace\4004A1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktotten\eclipse-workspace\4004A1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="178">
   <si>
     <t>yes/no</t>
   </si>
@@ -497,28 +497,133 @@
     <t>No</t>
   </si>
   <si>
-    <t>Line 61</t>
-  </si>
-  <si>
-    <t>Line 62</t>
-  </si>
-  <si>
-    <t>Line 64</t>
-  </si>
-  <si>
-    <t>Line 63</t>
-  </si>
-  <si>
-    <t>Lines 57-60</t>
-  </si>
-  <si>
     <t>DetectionTests/threeSuitTest</t>
   </si>
   <si>
     <t>DetectionTests/oneOffRoyalTest</t>
   </si>
   <si>
-    <t>Line 67</t>
+    <t>DetectionTests/inOrderRoyalFlushTest, DetectionTests/outOrderRoyalFlishTest, DetectionTests/failRoyalFlushTest</t>
+  </si>
+  <si>
+    <t>DetectionTests/inOrderStraightFlushTest, DetectionTests/outOrderStraightFlushTest, DetectionTests/failStraightFlushTest</t>
+  </si>
+  <si>
+    <t>DetectionTests/inOrderFourKindTest, DetectionTests/outOrderFourKindTest, DetectionTests/failFourKindTest</t>
+  </si>
+  <si>
+    <t>DetectionTests/inOrderFullHouseTest, DetectionTests/outOrderFullHouseTest, DetectionTests/failFullHouseTest</t>
+  </si>
+  <si>
+    <t>DetectionTests/inOrderFlushTest, DetectionTests/outOrderFlushTest, DetectionTests/failFlushTest</t>
+  </si>
+  <si>
+    <t>DetectionTests/inOrderStraightTest, DetectionTests/outOrderStraightTest, DetectionTests/failStraightTest</t>
+  </si>
+  <si>
+    <t>DetectionTests/threeKindTest</t>
+  </si>
+  <si>
+    <t>DetectionTests/twoPairTest</t>
+  </si>
+  <si>
+    <t>DetectionTests/pairTest</t>
+  </si>
+  <si>
+    <t>DetectionTests/independenceDetectionTest, SwapOneTests/flushOneSwapTest, SwapOneTests/straightOneSwapTest</t>
+  </si>
+  <si>
+    <t>DetectionTests/oppStraightAiNoTest, DetectionTests/neitherStraightTest, DetectionTests/bothStraightTest</t>
+  </si>
+  <si>
+    <t>SwapOneTests/flushOneSwapTest</t>
+  </si>
+  <si>
+    <t>Yes (only Tests)</t>
+  </si>
+  <si>
+    <t>All Tests in SwaplessWinTests/</t>
+  </si>
+  <si>
+    <t>Line 3: SwapZeroTests/fullHouseTest</t>
+  </si>
+  <si>
+    <t>Lines 57-60: SwappedWinTests/spadeRFvsHeartRF, SwappedWinTests/heartRFvsDiamondRF, SwappedWinTests/diamondRFvsClubRF, spadeRFvsClubRF</t>
+  </si>
+  <si>
+    <t>Line 61: SwappedWinTests/spadeSFvsHeartSF</t>
+  </si>
+  <si>
+    <t>Line 62: SwappedWinTests/spadeSFvsHigherSF</t>
+  </si>
+  <si>
+    <t>Line 63: SwappedWinTests/higherFourKind</t>
+  </si>
+  <si>
+    <t>Line 64: SwappedWinTests/higherFullHouse</t>
+  </si>
+  <si>
+    <t>Line 65: SwappedWinTests/higherStraightSuit</t>
+  </si>
+  <si>
+    <t>Line 66: SwappedWinTests/higherStraight</t>
+  </si>
+  <si>
+    <t>Line 67: SwappedWinTests/highestCard</t>
+  </si>
+  <si>
+    <t>Line 68: SwappedWinTests/highestCardSuit</t>
+  </si>
+  <si>
+    <t>Line 48: SwapZeroTests/StraightFlushTest</t>
+  </si>
+  <si>
+    <t>Line 57: SwapZeroTests/RoyalFlushTest</t>
+  </si>
+  <si>
+    <t>Line 42: SwapZeroTests/flushTest</t>
+  </si>
+  <si>
+    <t>Line 43: SwapZeroTests/straightTest</t>
+  </si>
+  <si>
+    <t>Line: 9 SwapOneTests/flushOneSwapTest</t>
+  </si>
+  <si>
+    <t>Line 10: SwapOneTests/straightOneSwapTest</t>
+  </si>
+  <si>
+    <t>Line 7: SwapOneTests/twoPairOneSwapTest</t>
+  </si>
+  <si>
+    <t>Line 11: SwapTwoTests/threeKindSwapTwoTest</t>
+  </si>
+  <si>
+    <t>Line 10: pairOverHigh</t>
+  </si>
+  <si>
+    <t>Lines 11-12: twoPairOverPair, twoPairOverHigh</t>
+  </si>
+  <si>
+    <t>Lines 13-15: threeKindOverTwoPair, threeKindOverPair, threeKindOverHigh</t>
+  </si>
+  <si>
+    <t>Lines 16-19: straightOverThreeKind, straightOverTwoPair, straightOverPair, straightOverHigh</t>
+  </si>
+  <si>
+    <t>Lines 20-24: flushOverStraight, flushOverThreeKind, straightOverTwoPair, straightOverPair, straightOverHigh</t>
+  </si>
+  <si>
+    <t>Lines 25-30: fullOverFlush, fullOverStraight, fullOverThreeKind, fullOverTwoPair, fullOverPair, fullOverHigh</t>
+  </si>
+  <si>
+    <t>Lines 31-37: fourKindOverFull, fourKindOverFlush, fourKindOverStraight, fourKindOverThreeKind, fourKindOverTwoPair, fourKindOverPair, fourKindOverHigh</t>
+  </si>
+  <si>
+    <t>Lines 38-45: straightFlushOverFourKind, straightFlushOverFull, straightFlushOverFlush, straightFlushOverStraight, straightFlushOverThreeKind, straightFlushOverTwoPair, straightFlushOverPair, straightFlushOverHigh</t>
+  </si>
+  <si>
+    <t>Lines 46-54: royalFlushOverStriaghtFlush, royalFlushOverFourKind, royalFlushOverFull, royalFlushOverFlush, royalFlushOverStraight, royalFlushOverThreeKind, royalFlushOverTwoPair, royalFlushOverPair, royalFlushOverHigh</t>
   </si>
 </sst>
 </file>
@@ -1453,8 +1558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1631,7 +1736,9 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1650,7 +1757,9 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1669,7 +1778,9 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1688,7 +1799,9 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1707,7 +1820,9 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1726,7 +1841,9 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1745,7 +1862,9 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1764,7 +1883,9 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1783,7 +1904,9 @@
       <c r="D22">
         <v>0.5</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1802,7 +1925,9 @@
       <c r="D23">
         <v>2</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1827,7 +1952,9 @@
       <c r="D25">
         <v>5</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1853,7 +1980,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1930,7 +2057,9 @@
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1969,7 +2098,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -1989,7 +2118,9 @@
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2027,7 +2158,9 @@
       <c r="D36">
         <v>1</v>
       </c>
-      <c r="E36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -2046,7 +2179,9 @@
       <c r="D37">
         <v>1</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -2093,7 +2228,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42">
@@ -2153,7 +2288,9 @@
       <c r="D48">
         <v>0.25</v>
       </c>
-      <c r="E48" s="2"/>
+      <c r="E48" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -2174,7 +2311,9 @@
       <c r="D49">
         <v>0.25</v>
       </c>
-      <c r="E49" s="2"/>
+      <c r="E49" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -2216,7 +2355,9 @@
       <c r="D51">
         <v>0.25</v>
       </c>
-      <c r="E51" s="2"/>
+      <c r="E51" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -2237,7 +2378,9 @@
       <c r="D52">
         <v>0.25</v>
       </c>
-      <c r="E52" s="2"/>
+      <c r="E52" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -2258,7 +2401,9 @@
       <c r="D53">
         <v>0.25</v>
       </c>
-      <c r="E53" s="2"/>
+      <c r="E53" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -2363,7 +2508,9 @@
       <c r="D58">
         <v>0.5</v>
       </c>
-      <c r="E58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>165</v>
+      </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -2378,13 +2525,15 @@
         <v>84</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59">
         <v>0.5</v>
       </c>
-      <c r="E59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>166</v>
+      </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -2426,7 +2575,9 @@
       <c r="D61">
         <v>0.25</v>
       </c>
-      <c r="E61" s="2"/>
+      <c r="E61" s="2" t="s">
+        <v>168</v>
+      </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -2468,7 +2619,9 @@
       <c r="D63">
         <v>0.5</v>
       </c>
-      <c r="E63" s="2"/>
+      <c r="E63" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -2528,6 +2681,9 @@
         <v>51</v>
       </c>
       <c r="C67"/>
+      <c r="E67" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
@@ -2540,7 +2696,9 @@
       <c r="D68">
         <v>0.25</v>
       </c>
-      <c r="E68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>177</v>
+      </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
@@ -2562,7 +2720,9 @@
       <c r="D69">
         <v>0.25</v>
       </c>
-      <c r="E69" s="2"/>
+      <c r="E69" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
@@ -2584,7 +2744,9 @@
       <c r="D70">
         <v>0.25</v>
       </c>
-      <c r="E70" s="2"/>
+      <c r="E70" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -2606,7 +2768,9 @@
       <c r="D71">
         <v>0.25</v>
       </c>
-      <c r="E71" s="2"/>
+      <c r="E71" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -2628,7 +2792,9 @@
       <c r="D72">
         <v>0.25</v>
       </c>
-      <c r="E72" s="2"/>
+      <c r="E72" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
@@ -2650,7 +2816,9 @@
       <c r="D73">
         <v>0.25</v>
       </c>
-      <c r="E73" s="2"/>
+      <c r="E73" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
@@ -2672,7 +2840,9 @@
       <c r="D74">
         <v>0.25</v>
       </c>
-      <c r="E74" s="2"/>
+      <c r="E74" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
@@ -2694,7 +2864,9 @@
       <c r="D75">
         <v>0.25</v>
       </c>
-      <c r="E75" s="2"/>
+      <c r="E75" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
@@ -2716,7 +2888,9 @@
       <c r="D76">
         <v>0.25</v>
       </c>
-      <c r="E76" s="2"/>
+      <c r="E76" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
@@ -2754,7 +2928,7 @@
         <v>0.5</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
@@ -2777,7 +2951,7 @@
         <v>0.5</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
@@ -2800,7 +2974,7 @@
         <v>0.5</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -2823,7 +2997,7 @@
         <v>0.5</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
@@ -2846,7 +3020,7 @@
         <v>0.5</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
@@ -2895,8 +3069,8 @@
       <c r="D87">
         <v>0.5</v>
       </c>
-      <c r="E87" s="2">
-        <v>66</v>
+      <c r="E87" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -2918,8 +3092,8 @@
       <c r="D88">
         <v>0.5</v>
       </c>
-      <c r="E88" s="2">
-        <v>65</v>
+      <c r="E88" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -3026,13 +3200,15 @@
         <v>36</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C96" s="6"/>
       <c r="D96">
         <v>0.5</v>
       </c>
-      <c r="E96" s="2"/>
+      <c r="E96" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
@@ -3059,7 +3235,7 @@
         <v>0.5</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>

</xml_diff>

<commit_message>
Admin Commit: Finalizing Files
</commit_message>
<xml_diff>
--- a/TottenKyle-grid.xlsx
+++ b/TottenKyle-grid.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -425,6 +425,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Regardless</t>
@@ -435,6 +436,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> of the positions of the cards in AIP's hand, you have tests that show you detect: </t>
@@ -665,6 +667,7 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -679,6 +682,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -687,6 +691,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -694,6 +699,7 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1558,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>